<commit_message>
map feature to US geometry
</commit_message>
<xml_diff>
--- a/data/utils/state_to_postal.xlsx
+++ b/data/utils/state_to_postal.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anmin/Documents/Courses/2023Winter/cs_app_2/final-project-ecoview/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anmin/Documents/Courses/2023Winter/cs_app_2/final-project-ecoview/data/utils/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{56532AFA-3E4D-1445-9639-FDCF2AF02190}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FD773AE-C20B-E74E-8D12-60AACFCA336E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="37260" yWindow="-1700" windowWidth="25380" windowHeight="16440" xr2:uid="{5698E13E-51BB-4146-A2AD-6CF08E11AFAC}"/>
   </bookViews>
@@ -122,9 +122,6 @@
     <t>DE</t>
   </si>
   <si>
-    <t>District of Columbia</t>
-  </si>
-  <si>
     <t>D.C.</t>
   </si>
   <si>
@@ -510,6 +507,9 @@
   </si>
   <si>
     <t>WY</t>
+  </si>
+  <si>
+    <t>District of Col.</t>
   </si>
 </sst>
 </file>
@@ -552,9 +552,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -873,630 +872,630 @@
   <dimension ref="A1:C56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="1" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
+      <c r="A11" t="s">
+        <v>158</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="C11" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="2" t="s">
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
+      <c r="B12" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="C12" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="2" t="s">
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
+      <c r="B13" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="C13" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C13" s="2" t="s">
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
+      <c r="B14" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C14" s="2" t="s">
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
+      <c r="B15" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C15" s="2" t="s">
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
+      <c r="B16" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C16" s="2" t="s">
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
+      <c r="B17" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="C17" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C17" s="2" t="s">
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
+      <c r="B18" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="C18" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C18" s="2" t="s">
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
+      <c r="B19" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C19" s="2" t="s">
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
+      <c r="B20" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="C20" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C20" s="2" t="s">
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
+      <c r="B21" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="C21" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C21" s="2" t="s">
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="2" t="s">
+      <c r="B22" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="C22" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C22" s="2" t="s">
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="2" t="s">
+      <c r="B23" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C23" s="2" t="s">
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="2" t="s">
+      <c r="B24" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="C24" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C24" s="2" t="s">
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="2" t="s">
+      <c r="B25" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="C25" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C25" s="2" t="s">
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="2" t="s">
+      <c r="B26" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="C26" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C26" s="2" t="s">
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="2" t="s">
+      <c r="B27" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="C27" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C27" s="2" t="s">
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" s="2" t="s">
+      <c r="B28" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="C28" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C28" s="2" t="s">
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" s="2" t="s">
+      <c r="B29" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="C29" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C29" s="2" t="s">
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" s="2" t="s">
+      <c r="B30" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="C30" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C30" s="2" t="s">
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" s="2" t="s">
+      <c r="B31" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="C31" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="C31" s="2" t="s">
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" s="2" t="s">
+      <c r="B32" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="C32" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C32" s="2" t="s">
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" s="2" t="s">
+      <c r="B33" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="C33" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C33" s="2" t="s">
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" s="2" t="s">
+      <c r="B34" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="C34" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="C34" s="2" t="s">
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" s="2" t="s">
+      <c r="B35" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="C35" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="C35" s="2" t="s">
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" s="2" t="s">
+      <c r="B36" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="C36" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C36" s="2" t="s">
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A37" s="2" t="s">
+      <c r="B37" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="C37" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="C37" s="2" t="s">
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A38" s="2" t="s">
+      <c r="B38" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="C38" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="C38" s="2" t="s">
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A39" s="2" t="s">
+      <c r="B39" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C39" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="B39" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="C39" s="2" t="s">
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A40" s="2" t="s">
+      <c r="B40" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="C40" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="C40" s="2" t="s">
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A41" s="2" t="s">
+      <c r="B41" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="C41" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="C41" s="2" t="s">
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A42" s="2" t="s">
+      <c r="B42" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="C42" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="C42" s="2" t="s">
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A43" s="2" t="s">
+      <c r="B43" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="C43" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="C43" s="2" t="s">
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A44" s="2" t="s">
+      <c r="B44" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="C44" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="C44" s="2" t="s">
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A45" s="2" t="s">
+      <c r="B45" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="C45" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="C45" s="2" t="s">
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" s="1" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A46" s="2" t="s">
+      <c r="B46" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="C46" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="C46" s="2" t="s">
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A47" s="2" t="s">
+      <c r="B47" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="C47" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="C47" s="2" t="s">
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" s="1" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A48" s="2" t="s">
+      <c r="B48" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C48" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="B48" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="C48" s="2" t="s">
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A49" s="2" t="s">
+      <c r="B49" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C49" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="B49" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="C49" s="2" t="s">
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" s="1" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A50" s="2" t="s">
+      <c r="B50" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="B50" s="2" t="s">
+      <c r="C50" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="C50" s="2" t="s">
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" s="1" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A51" s="2" t="s">
+      <c r="B51" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="C51" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="C51" s="2" t="s">
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" s="1" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A52" s="2" t="s">
+      <c r="B52" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="B52" s="2" t="s">
+      <c r="C52" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="C52" s="2" t="s">
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53" s="1" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A53" s="2" t="s">
+      <c r="B53" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="B53" s="2" t="s">
+      <c r="C53" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C53" s="2" t="s">
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54" s="1" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A54" s="2" t="s">
+      <c r="B54" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="B54" s="2" t="s">
+      <c r="C54" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="C54" s="2" t="s">
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55" s="1" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A55" s="2" t="s">
+      <c r="B55" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="B55" s="2" t="s">
+      <c r="C55" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="C55" s="2" t="s">
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56" s="1" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A56" s="2" t="s">
+      <c r="B56" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="B56" s="2" t="s">
+      <c r="C56" s="1" t="s">
         <v>157</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>158</v>
       </c>
     </row>
   </sheetData>

</xml_diff>